<commit_message>
Created a new backup bot. Will backup the database with memory storage in mind. Minor file cleanup aswell.
</commit_message>
<xml_diff>
--- a/Database/07_01.xlsx
+++ b/Database/07_01.xlsx
@@ -748,15 +748,6 @@
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
       <u val="none"/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -787,6 +778,15 @@
       <u val="none"/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1128,20 +1128,20 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="55">
       <alignment vertical="bottom" horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="56">
-      <alignment vertical="bottom" horizontal="left" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="25" xfId="0" numFmtId="187" borderId="0" applyFont="1" fontId="57" applyNumberFormat="1" applyFill="1">
+    <xf applyAlignment="1" fillId="25" xfId="0" numFmtId="187" borderId="0" applyFont="1" fontId="56" applyNumberFormat="1" applyFill="1">
       <alignment vertical="bottom" horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="58">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="57">
       <alignment vertical="bottom" horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="188" borderId="0" applyFont="1" fontId="59" applyNumberFormat="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="188" borderId="0" applyFont="1" fontId="58" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="59">
+      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="60">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
+      <alignment vertical="bottom" horizontal="left" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="26" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="61" applyFill="1">
       <alignment vertical="bottom" horizontal="right"/>
@@ -1273,7 +1273,7 @@
       <c s="24" r="X3"/>
     </row>
     <row r="4">
-      <c t="s" s="58" r="A4">
+      <c t="s" s="57" r="A4">
         <v>2</v>
       </c>
       <c s="24" r="B4"/>
@@ -1333,15 +1333,15 @@
         <f>HYPERLINK("http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J","http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J")</f>
         <v>http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J</v>
       </c>
-      <c s="58" r="B6"/>
-      <c s="58" r="C6"/>
-      <c s="58" r="D6"/>
-      <c s="58" r="E6"/>
-      <c s="58" r="F6"/>
-      <c s="58" r="G6"/>
-      <c s="58" r="H6"/>
-      <c s="58" r="I6"/>
-      <c s="58" r="J6"/>
+      <c s="57" r="B6"/>
+      <c s="57" r="C6"/>
+      <c s="57" r="D6"/>
+      <c s="57" r="E6"/>
+      <c s="57" r="F6"/>
+      <c s="57" r="G6"/>
+      <c s="57" r="H6"/>
+      <c s="57" r="I6"/>
+      <c s="57" r="J6"/>
       <c s="40" r="K6"/>
       <c s="40" r="L6"/>
       <c s="40" r="M6"/>
@@ -1362,12 +1362,12 @@
         <f>HYPERLINK("http://adsabs.harvard.edu/abs/2004PhyS...69..196J","http://adsabs.harvard.edu/abs/2004PhyS...69..196J")</f>
         <v>http://adsabs.harvard.edu/abs/2004PhyS...69..196J</v>
       </c>
-      <c s="58" r="B7"/>
-      <c s="58" r="C7"/>
-      <c s="58" r="D7"/>
-      <c s="58" r="E7"/>
-      <c s="58" r="F7"/>
-      <c s="58" r="G7"/>
+      <c s="57" r="B7"/>
+      <c s="57" r="C7"/>
+      <c s="57" r="D7"/>
+      <c s="57" r="E7"/>
+      <c s="57" r="F7"/>
+      <c s="57" r="G7"/>
       <c s="40" r="H7"/>
       <c s="40" r="I7"/>
       <c s="40" r="J7"/>
@@ -1391,12 +1391,12 @@
         <f>HYPERLINK("http://www.fisica.unam.mx/research/tables/spectra/1el/","http://www.fisica.unam.mx/research/tables/spectra/1el/")</f>
         <v>http://www.fisica.unam.mx/research/tables/spectra/1el/</v>
       </c>
-      <c s="58" r="B8"/>
-      <c s="58" r="C8"/>
-      <c s="58" r="D8"/>
-      <c s="58" r="E8"/>
-      <c s="58" r="F8"/>
-      <c s="58" r="G8"/>
+      <c s="57" r="B8"/>
+      <c s="57" r="C8"/>
+      <c s="57" r="D8"/>
+      <c s="57" r="E8"/>
+      <c s="57" r="F8"/>
+      <c s="57" r="G8"/>
       <c s="40" r="H8"/>
       <c s="40" r="I8"/>
       <c s="40" r="J8"/>
@@ -3703,14 +3703,14 @@
     <col min="13" customWidth="1" max="13" width="11.43"/>
     <col min="14" customWidth="1" max="14" style="13" width="11.43"/>
     <col min="15" customWidth="1" max="15" style="31" width="10.71"/>
-    <col min="16" customWidth="1" max="16" style="59" width="11.43"/>
-    <col min="17" customWidth="1" max="17" style="59" width="10.71"/>
-    <col min="18" customWidth="1" max="18" style="59" width="11.43"/>
-    <col min="19" customWidth="1" max="19" style="59" width="11.29"/>
-    <col min="20" customWidth="1" max="20" style="59" width="11.14"/>
-    <col min="21" max="21" style="59" width="12.29"/>
-    <col min="22" customWidth="1" max="22" style="59" width="10.86"/>
-    <col min="23" customWidth="1" max="23" style="59" width="10.43"/>
+    <col min="16" customWidth="1" max="16" style="58" width="11.43"/>
+    <col min="17" customWidth="1" max="17" style="58" width="10.71"/>
+    <col min="18" customWidth="1" max="18" style="58" width="11.43"/>
+    <col min="19" customWidth="1" max="19" style="58" width="11.29"/>
+    <col min="20" customWidth="1" max="20" style="58" width="11.14"/>
+    <col min="21" max="21" style="58" width="12.29"/>
+    <col min="22" customWidth="1" max="22" style="58" width="10.86"/>
+    <col min="23" customWidth="1" max="23" style="58" width="10.43"/>
     <col min="24" customWidth="1" max="25" width="11.29"/>
     <col min="26" customWidth="1" max="26" width="11.86"/>
     <col min="27" customWidth="1" max="27" width="9.0"/>
@@ -3847,16 +3847,16 @@
         <f>HYPERLINK("http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J","http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J")</f>
         <v>http://adsabs.harvard.edu/abs/2004JPCRD..33.1059J</v>
       </c>
-      <c s="58" r="B4"/>
-      <c s="58" r="C4"/>
-      <c s="58" r="D4"/>
-      <c s="58" r="E4"/>
-      <c s="58" r="F4"/>
-      <c s="58" r="G4"/>
-      <c s="58" r="H4"/>
-      <c s="58" r="I4"/>
-      <c s="58" r="J4"/>
-      <c s="58" r="K4"/>
+      <c s="57" r="B4"/>
+      <c s="57" r="C4"/>
+      <c s="57" r="D4"/>
+      <c s="57" r="E4"/>
+      <c s="57" r="F4"/>
+      <c s="57" r="G4"/>
+      <c s="57" r="H4"/>
+      <c s="57" r="I4"/>
+      <c s="57" r="J4"/>
+      <c s="57" r="K4"/>
       <c s="40" r="L4"/>
       <c s="40" r="M4"/>
       <c s="48" r="N4"/>
@@ -3889,13 +3889,13 @@
         <f>HYPERLINK("http://adsabs.harvard.edu/abs/2004PhyS...69..196J","http://adsabs.harvard.edu/abs/2004PhyS...69..196J")</f>
         <v>http://adsabs.harvard.edu/abs/2004PhyS...69..196J</v>
       </c>
-      <c s="58" r="B5"/>
-      <c s="58" r="C5"/>
-      <c s="58" r="D5"/>
-      <c s="58" r="E5"/>
-      <c s="58" r="F5"/>
-      <c s="58" r="G5"/>
-      <c s="58" r="H5"/>
+      <c s="57" r="B5"/>
+      <c s="57" r="C5"/>
+      <c s="57" r="D5"/>
+      <c s="57" r="E5"/>
+      <c s="57" r="F5"/>
+      <c s="57" r="G5"/>
+      <c s="57" r="H5"/>
       <c s="40" r="I5"/>
       <c s="40" r="J5"/>
       <c s="40" r="K5"/>
@@ -3931,13 +3931,13 @@
         <f>HYPERLINK("http://www.fisica.unam.mx/research/tables/spectra/1el/","http://www.fisica.unam.mx/research/tables/spectra/1el/")</f>
         <v>http://www.fisica.unam.mx/research/tables/spectra/1el/</v>
       </c>
-      <c s="58" r="B6"/>
-      <c s="58" r="C6"/>
-      <c s="58" r="D6"/>
-      <c s="58" r="E6"/>
-      <c s="58" r="F6"/>
-      <c s="58" r="G6"/>
-      <c s="58" r="H6"/>
+      <c s="57" r="B6"/>
+      <c s="57" r="C6"/>
+      <c s="57" r="D6"/>
+      <c s="57" r="E6"/>
+      <c s="57" r="F6"/>
+      <c s="57" r="G6"/>
+      <c s="57" r="H6"/>
       <c s="40" r="I6"/>
       <c s="40" r="J6"/>
       <c s="40" r="K6"/>
@@ -4358,7 +4358,7 @@
       <c t="s" s="44" r="D16">
         <v>18</v>
       </c>
-      <c t="s" s="57" r="E16">
+      <c t="s" s="56" r="E16">
         <v>52</v>
       </c>
       <c t="s" s="3" r="F16">
@@ -30574,7 +30574,7 @@
       <c s="24" r="V7"/>
     </row>
     <row customHeight="1" r="8" ht="12.0">
-      <c s="56" r="A8"/>
+      <c s="60" r="A8"/>
       <c s="55" r="B8"/>
       <c s="55" r="C8"/>
       <c s="55" r="D8"/>
@@ -30651,10 +30651,10 @@
       <c s="24" r="C11"/>
       <c s="24" r="D11"/>
       <c s="24" r="E11"/>
-      <c s="60" r="F11"/>
-      <c s="60" r="G11"/>
-      <c s="60" r="H11"/>
-      <c s="60" r="I11"/>
+      <c s="59" r="F11"/>
+      <c s="59" r="G11"/>
+      <c s="59" r="H11"/>
+      <c s="59" r="I11"/>
       <c s="24" r="J11"/>
       <c s="24" r="K11"/>
       <c s="24" r="L11"/>

</xml_diff>